<commit_message>
BOM error in line 51 corrected.
</commit_message>
<xml_diff>
--- a/cosmicpi_1.6_enhanced.xlsx
+++ b/cosmicpi_1.6_enhanced.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="663" uniqueCount="521">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="663" uniqueCount="523">
   <si>
     <t>Id;"Designator";"Package";"Quantity";"Designation";"Supplier and ref";</t>
   </si>
@@ -1610,6 +1610,12 @@
   </si>
   <si>
     <t>MPN (Manufacturer Part Number)</t>
+  </si>
+  <si>
+    <t>ERJ3EKF1000V</t>
+  </si>
+  <si>
+    <t>176-3495</t>
   </si>
 </sst>
 </file>
@@ -2111,7 +2117,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2124,6 +2130,8 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2454,8 +2462,8 @@
   </sheetPr>
   <dimension ref="A1:N62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2590,39 +2598,39 @@
         <v>413</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
         <f t="shared" ref="A4:A62" si="0">SUM(A3+1)</f>
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="8" t="s">
         <v>435</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="8" t="s">
         <v>444</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="8" t="s">
         <v>460</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="8" t="s">
         <v>443</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="8">
         <v>744235220</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="8">
         <v>2</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="8" t="s">
         <v>351</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="8" t="s">
         <v>352</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="8" t="s">
         <v>212</v>
       </c>
     </row>
@@ -3359,20 +3367,20 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="A27" s="8">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="8" t="s">
         <v>436</v>
       </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5" t="s">
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8" t="s">
         <v>437</v>
       </c>
-      <c r="G27" s="5">
+      <c r="G27" s="8">
         <v>2</v>
       </c>
       <c r="I27" s="6" t="s">
@@ -4160,7 +4168,7 @@
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52">
+      <c r="A52" s="5">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
@@ -4170,14 +4178,14 @@
       <c r="C52" t="s">
         <v>444</v>
       </c>
-      <c r="D52" t="s">
-        <v>515</v>
-      </c>
-      <c r="E52" t="s">
-        <v>455</v>
-      </c>
-      <c r="F52" t="s">
-        <v>420</v>
+      <c r="D52" s="5" t="s">
+        <v>522</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>459</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>521</v>
       </c>
       <c r="G52">
         <v>6</v>
@@ -4525,42 +4533,42 @@
         <v>341</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A62">
+    <row r="62" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="8">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="B62" s="8" t="s">
         <v>434</v>
       </c>
-      <c r="C62" s="5" t="s">
+      <c r="C62" s="8" t="s">
         <v>454</v>
       </c>
-      <c r="D62" s="5">
+      <c r="D62" s="8">
         <v>2380162</v>
       </c>
-      <c r="E62" s="5" t="s">
+      <c r="E62" s="8" t="s">
         <v>459</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F62" s="8" t="s">
         <v>432</v>
       </c>
-      <c r="G62" s="5">
+      <c r="G62" s="8">
         <v>5</v>
       </c>
-      <c r="H62" t="s">
+      <c r="H62" s="8" t="s">
         <v>433</v>
       </c>
-      <c r="J62" t="s">
+      <c r="J62" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="K62">
+      <c r="K62" s="8">
         <v>20</v>
       </c>
-      <c r="M62" s="1">
+      <c r="M62" s="9">
         <v>0.01</v>
       </c>
-      <c r="N62" t="s">
+      <c r="N62" s="8" t="s">
         <v>413</v>
       </c>
     </row>

</xml_diff>